<commit_message>
funcionando select de mes
</commit_message>
<xml_diff>
--- a/JLP_2025-01.xlsx
+++ b/JLP_2025-01.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -777,6 +777,34 @@
         </is>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Despesa</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>SERVIÇOS</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>100</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>30/01/2025</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>